<commit_message>
CL and WO Screen
</commit_message>
<xml_diff>
--- a/Doc/LOAN_WO.xlsx
+++ b/Doc/LOAN_WO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>WO_AMOUNT</t>
   </si>
@@ -77,6 +77,30 @@
   </si>
   <si>
     <t>SME</t>
+  </si>
+  <si>
+    <t>PRODUCT_CODE</t>
+  </si>
+  <si>
+    <t>PRODUCT_DESC</t>
+  </si>
+  <si>
+    <t>EBL-TWO WHEELER</t>
+  </si>
+  <si>
+    <t>0749</t>
+  </si>
+  <si>
+    <t>LOAN_AC_NUMBER</t>
+  </si>
+  <si>
+    <t>3011380057880</t>
+  </si>
+  <si>
+    <t>0031010025874</t>
+  </si>
+  <si>
+    <t>0041010006371</t>
   </si>
 </sst>
 </file>
@@ -476,10 +500,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,13 +511,13 @@
     <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="2" customWidth="1"/>
-    <col min="4" max="6" width="29.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="4" max="9" width="29.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -512,17 +536,26 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -541,17 +574,26 @@
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="4">
         <v>2000</v>
       </c>
-      <c r="H2" s="4">
+      <c r="K2" s="4">
         <v>1000</v>
       </c>
-      <c r="I2" s="6">
+      <c r="L2" s="6">
         <v>44196</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -570,17 +612,26 @@
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="4">
         <v>1500</v>
       </c>
-      <c r="H3" s="4">
+      <c r="K3" s="4">
         <v>1500</v>
       </c>
-      <c r="I3" s="6">
+      <c r="L3" s="6">
         <v>44196</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -599,13 +650,22 @@
       <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="4">
         <v>1200</v>
       </c>
-      <c r="H4" s="4">
+      <c r="K4" s="4">
         <v>2000</v>
       </c>
-      <c r="I4" s="6">
+      <c r="L4" s="6">
         <v>44196</v>
       </c>
     </row>

</xml_diff>